<commit_message>
dashboard RH commit 03
</commit_message>
<xml_diff>
--- a/arquivos/PowerBI + SQLServer/1_MODULO - POWER_BI - Starter/1_RH/SALARIOS.xlsx
+++ b/arquivos/PowerBI + SQLServer/1_MODULO - POWER_BI - Starter/1_RH/SALARIOS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319B1E99-A01E-4ABF-BAD5-8148E9282866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC9DC08-C315-4CC0-B072-76A3B36A843E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24105" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -59,19 +59,10 @@
     <t>IDADE</t>
   </si>
   <si>
-    <t>25</t>
-  </si>
-  <si>
     <t>14/02/2019</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>11</t>
-  </si>
-  <si>
-    <t>8000</t>
   </si>
   <si>
     <t>15</t>
@@ -472,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -600,6 +591,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1567,7 +1561,7 @@
   <sheetData>
     <row r="5" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
@@ -1575,7 +1569,7 @@
       <c r="F5" s="26"/>
       <c r="G5" s="27"/>
       <c r="I5" s="43" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J5" s="43"/>
       <c r="K5" s="43"/>
@@ -1597,7 +1591,7 @@
       <c r="F7" s="29"/>
       <c r="G7" s="30"/>
       <c r="I7" s="31" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
@@ -1605,7 +1599,7 @@
     </row>
     <row r="8" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="34" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
@@ -1628,7 +1622,7 @@
       <c r="F9" s="38"/>
       <c r="G9" s="39"/>
       <c r="I9" s="31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
@@ -1660,7 +1654,7 @@
       <c r="F11" s="38"/>
       <c r="G11" s="39"/>
       <c r="I11" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
@@ -1692,7 +1686,7 @@
       <c r="F13" s="38"/>
       <c r="G13" s="39"/>
       <c r="I13" s="31" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
@@ -1724,7 +1718,7 @@
       <c r="F15" s="38"/>
       <c r="G15" s="39"/>
       <c r="I15" s="31" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J15" s="32"/>
       <c r="K15" s="32"/>
@@ -1784,7 +1778,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1814,28 +1808,28 @@
         <v>9</v>
       </c>
       <c r="D1" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>31</v>
       </c>
       <c r="F1" s="24" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H1" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="24" t="s">
-        <v>21</v>
-      </c>
       <c r="J1" s="24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1843,7 +1837,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2" s="15">
         <v>19</v>
@@ -1852,7 +1846,7 @@
         <v>43501</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F2" s="17">
         <v>2000</v>
@@ -1864,10 +1858,10 @@
         <v>6</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K2" s="19">
         <v>6</v>
@@ -1878,7 +1872,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C3" s="8">
         <v>50</v>
@@ -1887,7 +1881,7 @@
         <v>43502</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F3" s="8">
         <v>8000</v>
@@ -1899,10 +1893,10 @@
         <v>6</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K3" s="12">
         <v>3</v>
@@ -1922,7 +1916,7 @@
         <v>43503</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F4" s="8">
         <v>7000</v>
@@ -1934,10 +1928,10 @@
         <v>6</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K4" s="12">
         <v>0</v>
@@ -1957,7 +1951,7 @@
         <v>43504</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F5" s="8">
         <v>3588</v>
@@ -1969,10 +1963,10 @@
         <v>7</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K5" s="12">
         <v>2</v>
@@ -1983,7 +1977,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6" s="8">
         <v>55</v>
@@ -1992,7 +1986,7 @@
         <v>43505</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F6" s="8">
         <v>5600</v>
@@ -2004,10 +1998,10 @@
         <v>7</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K6" s="12">
         <v>2</v>
@@ -2015,34 +2009,34 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="44">
+        <v>25</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="E7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="F7" s="44">
+        <v>8000</v>
+      </c>
+      <c r="G7" s="44">
+        <v>0</v>
       </c>
       <c r="H7" s="13" t="s">
         <v>6</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K7" s="12">
         <v>4</v>
@@ -2053,7 +2047,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C8" s="8">
         <v>21</v>
@@ -2062,7 +2056,7 @@
         <v>43506</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F8" s="8">
         <v>1800</v>
@@ -2074,10 +2068,10 @@
         <v>7</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K8" s="12">
         <v>1</v>
@@ -2088,7 +2082,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C9" s="8">
         <v>65</v>
@@ -2097,7 +2091,7 @@
         <v>43507</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F9" s="10">
         <v>2500</v>
@@ -2109,10 +2103,10 @@
         <v>7</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K9" s="12">
         <v>1</v>
@@ -2123,7 +2117,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C10" s="8">
         <v>45</v>
@@ -2132,7 +2126,7 @@
         <v>43508</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F10" s="10">
         <v>3000</v>
@@ -2144,10 +2138,10 @@
         <v>7</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K10" s="12">
         <v>1</v>
@@ -2167,7 +2161,7 @@
         <v>43509</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F11" s="8">
         <v>3000</v>
@@ -2179,10 +2173,10 @@
         <v>7</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K11" s="12">
         <v>0</v>
@@ -2202,7 +2196,7 @@
         <v>43538</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F12" s="8">
         <v>2300</v>
@@ -2214,10 +2208,10 @@
         <v>6</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K12" s="12">
         <v>0</v>
@@ -2225,10 +2219,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C13" s="8">
         <v>33</v>
@@ -2237,7 +2231,7 @@
         <v>43510</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F13" s="8">
         <v>12000</v>
@@ -2249,10 +2243,10 @@
         <v>7</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K13" s="12">
         <v>2</v>
@@ -2263,7 +2257,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C14" s="8">
         <v>26</v>
@@ -2272,7 +2266,7 @@
         <v>43511</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F14" s="8">
         <v>15000</v>
@@ -2284,10 +2278,10 @@
         <v>7</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K14" s="12">
         <v>0</v>
@@ -2298,7 +2292,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C15" s="8">
         <v>29</v>
@@ -2307,7 +2301,7 @@
         <v>43512</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F15" s="8">
         <v>14000</v>
@@ -2319,10 +2313,10 @@
         <v>7</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K15" s="12">
         <v>0</v>
@@ -2333,7 +2327,7 @@
         <v>171</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C16" s="8">
         <v>26</v>
@@ -2342,7 +2336,7 @@
         <v>43512</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F16" s="8">
         <v>8000</v>
@@ -2354,10 +2348,10 @@
         <v>6</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K16" s="12">
         <v>3</v>
@@ -2368,7 +2362,7 @@
         <v>523</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C17" s="8">
         <v>21</v>
@@ -2377,7 +2371,7 @@
         <v>43512</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F17" s="8">
         <v>1500</v>
@@ -2389,10 +2383,10 @@
         <v>7</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K17" s="12">
         <v>2</v>
@@ -2403,7 +2397,7 @@
         <v>555</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" s="8">
         <v>28</v>
@@ -2412,7 +2406,7 @@
         <v>43512</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F18" s="8">
         <v>4500</v>
@@ -2424,10 +2418,10 @@
         <v>7</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K18" s="12">
         <v>1</v>
@@ -2438,7 +2432,7 @@
         <v>369</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C19" s="8">
         <v>29</v>
@@ -2447,7 +2441,7 @@
         <v>43512</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F19" s="8">
         <v>4000</v>
@@ -2459,10 +2453,10 @@
         <v>6</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K19" s="12">
         <v>1</v>
@@ -2470,10 +2464,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C20" s="8">
         <v>26</v>
@@ -2482,7 +2476,7 @@
         <v>43512</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F20" s="8">
         <v>3500</v>
@@ -2491,13 +2485,13 @@
         <v>0</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K20" s="12">
         <v>5</v>
@@ -2505,10 +2499,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C21" s="8">
         <v>23</v>
@@ -2517,7 +2511,7 @@
         <v>43512</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F21" s="8">
         <v>4500</v>
@@ -2526,13 +2520,13 @@
         <v>0</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K21" s="12">
         <v>0</v>

</xml_diff>